<commit_message>
updating the cost estimate
</commit_message>
<xml_diff>
--- a/Docs/Costestimation.xlsx
+++ b/Docs/Costestimation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533908\Desktop\PM Milestone\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533908\Desktop\project_management_controller\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279976C1-29B4-4FB7-956A-C5D9C6ABA583}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C21B2A1-F871-4737-B82A-F25B31D55C76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -569,13 +569,13 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.42578125" customWidth="1"/>
-    <col min="2" max="2" width="54.5703125" customWidth="1"/>
+    <col min="2" max="2" width="71.5703125" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
     <col min="4" max="4" width="13.140625" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" customWidth="1"/>

</xml_diff>